<commit_message>
Returns the name and score of the latest test a student took.
</commit_message>
<xml_diff>
--- a/A4P3/scores.xlsx
+++ b/A4P3/scores.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deeprajpandey/Desktop/Computer Networks/hw4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deeprajpandey/Desktop/Computer Networks/networks/A4P3/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="monsoon19" sheetId="1" r:id="rId1"/>
@@ -47,31 +47,31 @@
     <t>yash.dixit_ug20</t>
   </si>
   <si>
-    <t>students</t>
-  </si>
-  <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>test3</t>
-  </si>
-  <si>
-    <t>midterm</t>
-  </si>
-  <si>
-    <t>test4</t>
-  </si>
-  <si>
-    <t>test5</t>
-  </si>
-  <si>
-    <t>test6</t>
-  </si>
-  <si>
-    <t>final</t>
+    <t>Students</t>
+  </si>
+  <si>
+    <t>test 1</t>
+  </si>
+  <si>
+    <t>Test 2</t>
+  </si>
+  <si>
+    <t>Test 3</t>
+  </si>
+  <si>
+    <t>Midterm</t>
+  </si>
+  <si>
+    <t>Test 4</t>
+  </si>
+  <si>
+    <t>Test 5</t>
+  </si>
+  <si>
+    <t>Test 6</t>
+  </si>
+  <si>
+    <t>Final</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -480,9 +480,6 @@
       <c r="H3">
         <v>30</v>
       </c>
-      <c r="I3">
-        <v>25</v>
-      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">

</xml_diff>

<commit_message>
Added a sheet to store passwords: all initialised to not set
</commit_message>
<xml_diff>
--- a/A4P3/scores.xlsx
+++ b/A4P3/scores.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="monsoon19" sheetId="1" r:id="rId1"/>
+    <sheet name="passwords" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>archit.checker_ug20</t>
   </si>
@@ -72,6 +73,12 @@
   </si>
   <si>
     <t>Final</t>
+  </si>
+  <si>
+    <t>not set</t>
+  </si>
+  <si>
+    <t>stored</t>
   </si>
 </sst>
 </file>
@@ -388,8 +395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -600,4 +607,63 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Moved password management into a json file from excel
</commit_message>
<xml_diff>
--- a/A4P3/scores.xlsx
+++ b/A4P3/scores.xlsx
@@ -9,11 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="monsoon19" sheetId="1" r:id="rId1"/>
-    <sheet name="passwords" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>archit.checker_ug20</t>
   </si>
@@ -73,12 +72,6 @@
   </si>
   <si>
     <t>Final</t>
-  </si>
-  <si>
-    <t>not set</t>
-  </si>
-  <si>
-    <t>stored</t>
   </si>
 </sst>
 </file>
@@ -395,8 +388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -607,63 +600,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="18.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Some variety in scores
</commit_message>
<xml_diff>
--- a/A4P3/scores.xlsx
+++ b/A4P3/scores.xlsx
@@ -389,7 +389,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -561,12 +561,6 @@
       <c r="G6">
         <v>22</v>
       </c>
-      <c r="H6">
-        <v>21</v>
-      </c>
-      <c r="I6">
-        <v>25</v>
-      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">

</xml_diff>